<commit_message>
Validate list of files
</commit_message>
<xml_diff>
--- a/openn/tests/data/sheets/pages_invalid.xlsx
+++ b/openn/tests/data/sheets/pages_invalid.xlsx
@@ -1755,9 +1755,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J42" sqref="J42"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B102" sqref="B102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -4171,8 +4171,8 @@
         <v>383</v>
       </c>
     </row>
-    <row r="102" spans="2:10">
-      <c r="B102" s="3">
+    <row r="102" spans="2:10" ht="15">
+      <c r="B102" s="10">
         <v>99</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Validate uniqueness within repeating values
</commit_message>
<xml_diff>
--- a/openn/tests/data/sheets/pages_invalid.xlsx
+++ b/openn/tests/data/sheets/pages_invalid.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25823"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="11440" yWindow="1120" windowWidth="25600" windowHeight="16060" activeTab="2"/>
+    <workbookView xWindow="11440" yWindow="1120" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="Pages" sheetId="4" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="386">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="385">
   <si>
     <t>1r</t>
   </si>
@@ -1196,9 +1196,6 @@
   </si>
   <si>
     <t>December 12</t>
-  </si>
-  <si>
-    <t>HelenGriffith_BMC_0093.tif</t>
   </si>
   <si>
     <t>HelenGriffith_BMC_0094.tif</t>
@@ -1332,7 +1329,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="53">
+  <cellStyleXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1386,6 +1383,8 @@
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1402,7 +1401,7 @@
     <xf numFmtId="49" fontId="8" fillId="5" borderId="0" xfId="50" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="7" fillId="4" borderId="0" xfId="49" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="53">
+  <cellStyles count="55">
     <cellStyle name="Bad" xfId="50" builtinId="27"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -1432,6 +1431,7 @@
     <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="49" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
@@ -1454,6 +1454,7 @@
     <cellStyle name="Hyperlink" xfId="38" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="40" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="15"/>
   </cellStyles>
@@ -1756,9 +1757,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L102"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B102" sqref="B102"/>
+      <selection pane="bottomLeft" activeCell="D98" sqref="D98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2233,7 +2234,7 @@
       </c>
       <c r="K21" s="9"/>
       <c r="L21" s="11" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="22" spans="2:12">
@@ -2711,7 +2712,7 @@
         <v>198</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="J42" s="12" t="s">
         <v>199</v>
@@ -4128,15 +4129,15 @@
         <v>379</v>
       </c>
     </row>
-    <row r="98" spans="2:10">
+    <row r="98" spans="2:10" ht="15">
       <c r="B98" s="3">
         <v>95</v>
       </c>
       <c r="C98" t="s">
         <v>92</v>
       </c>
-      <c r="D98" t="s">
-        <v>380</v>
+      <c r="D98" s="11" t="s">
+        <v>377</v>
       </c>
     </row>
     <row r="99" spans="2:10">
@@ -4147,7 +4148,7 @@
         <v>93</v>
       </c>
       <c r="D99" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="100" spans="2:10">
@@ -4158,7 +4159,7 @@
         <v>94</v>
       </c>
       <c r="D100" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="101" spans="2:10">
@@ -4169,7 +4170,7 @@
         <v>95</v>
       </c>
       <c r="D101" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="102" spans="2:10" ht="15">
@@ -4305,7 +4306,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>

</xml_diff>